<commit_message>
Acrescentando a ligação da vulnerabilidade do SWC-112 para o DASP-2
</commit_message>
<xml_diff>
--- a/mythril/teste_0.24.7_smartbugs-curated/acurado.xlsx
+++ b/mythril/teste_0.24.7_smartbugs-curated/acurado.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="3">
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -599,19 +599,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9">
@@ -671,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>

</xml_diff>